<commit_message>
Update on 20200427 part 2
</commit_message>
<xml_diff>
--- a/文档/测试工作相关/IT端到端测试相关/测试内容相关/2020/20200423/鹏博士合作宽带根产品开发需求(206322063)/鹏博士合作宽带根产品开发需求(206322063)测试结果.xlsx
+++ b/文档/测试工作相关/IT端到端测试相关/测试内容相关/2020/20200423/鹏博士合作宽带根产品开发需求(206322063)/鹏博士合作宽带根产品开发需求(206322063)测试结果.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>序号</t>
   </si>
@@ -106,64 +106,109 @@
     <t>备注</t>
   </si>
   <si>
+    <t>新增鹏博士宽带产品，IBP开通流程参照有线宽带（524），当订单中含有省高清业务（ITV）子产品时”参照有线宽带（524）带子产品后付费宽带拨号IPTV 4K类  ，需要派发iptv工单，外线。需要通知客保系统新增此产品。</t>
+  </si>
+  <si>
+    <t>张君</t>
+  </si>
+  <si>
+    <t>产品管理处</t>
+  </si>
+  <si>
+    <t>鹏博士合作宽带根产品开发需求</t>
+  </si>
+  <si>
+    <t>为发展鹏博士合作宽带业务，现需在CRM新增“鹏博士合作”宽带拨号产品，包括预付费、后付费，宽带设备号为PBS开头，上网账号以ad9开头（与NOC确认单独规划，先从ad90000001-ad90499999），涉及到的宽带包月种类、子产品（含一次性费用）详见附件。目前仅开放住宅价格表，不开放受理政企价格表。</t>
+  </si>
+  <si>
+    <t>2020.04.28</t>
+  </si>
+  <si>
+    <t>预付费鹏博士宽带带省高清业务（ITV）子产品新装</t>
+  </si>
+  <si>
+    <t>预付费鹏博士宽带改性能升速</t>
+  </si>
+  <si>
+    <t>预付费鹏博士宽带（含省高清业务（ITV）子产品）移机</t>
+  </si>
+  <si>
+    <t>预付费鹏博士宽带（含省高清业务（ITV）子产品）拆机</t>
+  </si>
+  <si>
+    <t>问题序号</t>
+  </si>
+  <si>
+    <t>CRM订单号</t>
+  </si>
+  <si>
+    <t>发现BUG时间</t>
+  </si>
+  <si>
+    <t>BUG描述</t>
+  </si>
+  <si>
+    <t>BUG系统</t>
+  </si>
+  <si>
+    <t>BUG状态</t>
+  </si>
+  <si>
+    <t>BUG解决时间</t>
+  </si>
+  <si>
+    <t>bug分类</t>
+  </si>
+  <si>
+    <t>WMX2020042605389540</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试通过</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
     <t>预付费鹏博士宽带新装</t>
-  </si>
-  <si>
-    <t>新增鹏博士宽带产品，IBP开通流程参照有线宽带（524），当订单中含有省高清业务（ITV）子产品时”参照有线宽带（524）带子产品后付费宽带拨号IPTV 4K类  ，需要派发iptv工单，外线。需要通知客保系统新增此产品。</t>
-  </si>
-  <si>
-    <t>张君</t>
-  </si>
-  <si>
-    <t>产品管理处</t>
-  </si>
-  <si>
-    <t>鹏博士合作宽带根产品开发需求</t>
-  </si>
-  <si>
-    <t>为发展鹏博士合作宽带业务，现需在CRM新增“鹏博士合作”宽带拨号产品，包括预付费、后付费，宽带设备号为PBS开头，上网账号以ad9开头（与NOC确认单独规划，先从ad90000001-ad90499999），涉及到的宽带包月种类、子产品（含一次性费用）详见附件。目前仅开放住宅价格表，不开放受理政企价格表。</t>
-  </si>
-  <si>
-    <t>2020.04.28</t>
-  </si>
-  <si>
-    <t>预付费鹏博士宽带带省高清业务（ITV）子产品新装</t>
-  </si>
-  <si>
-    <t>预付费鹏博士宽带改性能升速</t>
-  </si>
-  <si>
-    <t>预付费鹏博士宽带（含省高清业务（ITV）子产品）移机</t>
-  </si>
-  <si>
-    <t>预付费鹏博士宽带（含省高清业务（ITV）子产品）拆机</t>
-  </si>
-  <si>
-    <t>问题序号</t>
-  </si>
-  <si>
-    <t>CRM订单号</t>
-  </si>
-  <si>
-    <t>发现BUG时间</t>
-  </si>
-  <si>
-    <t>BUG描述</t>
-  </si>
-  <si>
-    <t>BUG系统</t>
-  </si>
-  <si>
-    <t>BUG状态</t>
-  </si>
-  <si>
-    <t>BUG解决时间</t>
-  </si>
-  <si>
-    <t>bug分类</t>
-  </si>
-  <si>
-    <t>测试通过/不通过</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>预付费鹏博士宽带新装</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>环境问题</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>IBP</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单从CRM受理提交到IBP后，从SOP发送订单到P7系统未成功</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>WMX2020042705390546</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>WMX2020042705390547</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>WMX2020042705390821</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>WMX2020042705390832</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>WMX2020042705390877</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1004,7 +1049,7 @@
       <c r="IR1" s="23"/>
       <c r="IS1" s="23"/>
     </row>
-    <row r="2" spans="1:253" ht="48.95" customHeight="1">
+    <row r="2" spans="1:253" ht="24">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -1012,40 +1057,42 @@
         <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E2" s="15"/>
       <c r="F2" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="25">
         <v>5</v>
       </c>
       <c r="H2" s="27"/>
       <c r="I2" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>22</v>
       </c>
       <c r="K2" s="28">
         <v>206301121</v>
       </c>
       <c r="L2" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="29" t="s">
         <v>23</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>24</v>
       </c>
       <c r="N2" s="28"/>
       <c r="O2" s="28"/>
       <c r="P2" s="27"/>
       <c r="Q2" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R2" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S2" s="30"/>
       <c r="T2" s="24"/>
@@ -1283,7 +1330,7 @@
       <c r="IR2" s="24"/>
       <c r="IS2" s="24"/>
     </row>
-    <row r="3" spans="1:253" ht="36">
+    <row r="3" spans="1:253" ht="39.950000000000003" customHeight="1">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -1291,9 +1338,11 @@
         <v>38</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="E3" s="15"/>
       <c r="F3" s="26"/>
       <c r="G3" s="25"/>
@@ -1544,7 +1593,7 @@
       <c r="IR3" s="24"/>
       <c r="IS3" s="24"/>
     </row>
-    <row r="4" spans="1:253" ht="45.95" customHeight="1">
+    <row r="4" spans="1:253" ht="24">
       <c r="A4" s="20">
         <v>3</v>
       </c>
@@ -1552,9 +1601,11 @@
         <v>38</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E4" s="15"/>
       <c r="F4" s="26"/>
       <c r="G4" s="25"/>
@@ -1805,7 +1856,7 @@
       <c r="IR4" s="24"/>
       <c r="IS4" s="24"/>
     </row>
-    <row r="5" spans="1:253" ht="42" customHeight="1">
+    <row r="5" spans="1:253" ht="36">
       <c r="A5" s="20">
         <v>4</v>
       </c>
@@ -1813,9 +1864,11 @@
         <v>38</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="E5" s="15"/>
       <c r="F5" s="26"/>
       <c r="G5" s="25"/>
@@ -2066,7 +2119,7 @@
       <c r="IR5" s="24"/>
       <c r="IS5" s="24"/>
     </row>
-    <row r="6" spans="1:253" ht="42.95" customHeight="1">
+    <row r="6" spans="1:253" ht="36">
       <c r="A6" s="20">
         <v>5</v>
       </c>
@@ -2074,9 +2127,11 @@
         <v>38</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="E6" s="15"/>
       <c r="F6" s="26"/>
       <c r="G6" s="25"/>
@@ -2360,59 +2415,77 @@
     <col min="1" max="1" width="8.25" style="3"/>
     <col min="2" max="2" width="19.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.75" style="5" customWidth="1"/>
     <col min="7" max="7" width="8.25" style="1"/>
     <col min="8" max="8" width="11.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="4" customWidth="1"/>
+    <col min="9" max="9" width="16.875" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.375" style="1" customWidth="1"/>
     <col min="11" max="16384" width="8.25" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="36">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="D2" s="11">
+        <v>43947.465277777781</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>42</v>
+      </c>
       <c r="H2" s="15"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="5"/>
+      <c r="I2" s="11">
+        <v>43947.579861111109</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="10"/>

</xml_diff>